<commit_message>
Fix error in axis
</commit_message>
<xml_diff>
--- a/Levenshtein Distance/Levensthein.xlsx
+++ b/Levenshtein Distance/Levensthein.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Sj\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Sj\Desktop\Github\CX4034-TF-IDF-Generator\Levenshtein Distance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B63066C-58FE-4A84-BEBC-6237536B0304}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EEECE14-97C4-4FAA-A513-A6DDAF0C31BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B03B7C46-EF11-4176-A401-3ED84672E0F4}"/>
   </bookViews>
@@ -119,25 +119,18 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -457,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02ABC689-50F3-4209-9366-4E7901DC12A7}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,478 +460,478 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+      <c r="F5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3">
         <v>0</v>
       </c>
-      <c r="C6" s="4">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4">
-        <v>2</v>
-      </c>
-      <c r="E6" s="4">
-        <v>3</v>
-      </c>
-      <c r="F6" s="4">
-        <v>4</v>
-      </c>
-      <c r="G6" s="4">
-        <v>5</v>
-      </c>
-      <c r="H6" s="4">
-        <v>6</v>
-      </c>
-      <c r="I6" s="4">
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>3</v>
+      </c>
+      <c r="F6" s="3">
+        <v>4</v>
+      </c>
+      <c r="G6" s="3">
+        <v>5</v>
+      </c>
+      <c r="H6" s="3">
+        <v>6</v>
+      </c>
+      <c r="I6" s="3">
         <v>7</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="3">
         <v>8</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="3">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4">
-        <f>MIN(C6+$C$3, B7+$D$3, IF(C$5=$A7,B6+0,B6+$E$3))</f>
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <f>MIN(C6+$D$3, B7+$C$3, IF(C$5=$A7,B6+0,B6+$E$3))</f>
         <v>0</v>
       </c>
-      <c r="D7" s="4">
-        <f t="shared" ref="D7:K15" si="0">MIN(D6+$C$3, C7+$D$3, IF(D$5=$A7,C6+0,C6+$E$3))</f>
-        <v>1</v>
-      </c>
-      <c r="E7" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F7" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G7" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H7" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="I7" s="4">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="J7" s="4">
+      <c r="D7" s="3">
+        <f t="shared" ref="D7:K15" si="0">MIN(D6+$D$3, C7+$C$3, IF(D$5=$A7,C6+0,C6+$E$3))</f>
+        <v>1</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H7" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="J7" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="4">
-        <v>2</v>
-      </c>
-      <c r="C8" s="4">
-        <f t="shared" ref="C8:C15" si="1">MIN(C7+$C$3, B8+$D$3, IF(C$5=$A8,B7+0,B7+$E$3))</f>
-        <v>1</v>
-      </c>
-      <c r="D8" s="4">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E8" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F8" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G8" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H8" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="I8" s="4">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="J8" s="4">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" ref="C8:C15" si="1">MIN(C7+$D$3, B8+$C$3, IF(C$5=$A8,B7+0,B7+$E$3))</f>
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H8" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="J8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="4">
-        <v>3</v>
-      </c>
-      <c r="C9" s="4">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3">
+        <v>3</v>
+      </c>
+      <c r="C9" s="3">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="D9" s="4">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E9" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F9" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G9" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H9" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="I9" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="J9" s="4">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="K9" s="4">
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K9" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="4">
-        <v>4</v>
-      </c>
-      <c r="C10" s="4">
+      <c r="B10" s="3">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D10" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E10" s="4">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F10" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G10" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H10" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="I10" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="J10" s="4">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="K10" s="4">
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K10" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="4">
-        <v>5</v>
-      </c>
-      <c r="C11" s="4">
+      <c r="B11" s="3">
+        <v>5</v>
+      </c>
+      <c r="C11" s="3">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="D11" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="E11" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F11" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G11" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H11" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="I11" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="J11" s="4">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="K11" s="4">
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H11" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I11" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K11" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="4">
-        <v>6</v>
-      </c>
-      <c r="C12" s="4">
+      <c r="A12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="D12" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E12" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F12" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G12" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H12" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I12" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="J12" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="K12" s="4">
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H12" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I12" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K12" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3">
         <v>7</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="D13" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E13" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="F13" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G13" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H13" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I13" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="J13" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="K13" s="4">
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H13" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I13" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J13" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="K13" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3">
         <v>8</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="D14" s="4">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="E14" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="F14" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="G14" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H14" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="I14" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="J14" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="K14" s="4">
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H14" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I14" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K14" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3">
         <v>9</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="E15" s="4">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="F15" s="4">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G15" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="H15" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="I15" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="J15" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="K15" s="4">
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H15" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="I15" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J15" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K15" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>

</xml_diff>